<commit_message>
new changes for pbi exec
</commit_message>
<xml_diff>
--- a/src/b4d_pbi_executive_dashboard/src/b4d_currency_closing.xlsx
+++ b/src/b4d_pbi_executive_dashboard/src/b4d_currency_closing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\b4d\projects\b4d_analytics\src\b4d_pbi_executive_dashboard\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FEBB814-0BA4-47AC-9071-5B25830AD119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F5FAF7-B0AF-41D6-A747-C81E5FC620C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="2985" windowWidth="19005" windowHeight="9585" xr2:uid="{005786F0-4B55-4B6E-8711-110351EA8249}"/>
+    <workbookView xWindow="8460" yWindow="4410" windowWidth="19005" windowHeight="9585" xr2:uid="{005786F0-4B55-4B6E-8711-110351EA8249}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="5">
   <si>
     <t>USD</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>BS</t>
   </si>
 </sst>
 </file>
@@ -389,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22543093-2AE0-4CAE-9CC8-975B72734978}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C14" sqref="C14:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,6 +543,138 @@
         <v>26</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45658</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45689</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45717</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45748</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45778</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45809</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>45839</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45870</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>45901</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>45931</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>45962</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>45992</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>